<commit_message>
01/12 WLOP doc edit
</commit_message>
<xml_diff>
--- a/WLOP_project01/테스트 케이스.xlsx
+++ b/WLOP_project01/테스트 케이스.xlsx
@@ -5,11 +5,11 @@
   <x:workbookPr date1904="0" showBorderUnselectedTables="1" filterPrivacy="0" promptedSolutions="0" showInkAnnotation="1" backupFile="0" saveExternalLinkValues="1" codeName="ThisWorkbook" hidePivotFieldList="0" allowRefreshQuery="0" publishItems="0" checkCompatibility="0" autoCompressPictures="1" refreshAllConnections="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Desktop\한화 BEYOND SW\단위프로젝트1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Desktop\HW BEYOND SW\WLOP_project01\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <x:bookViews>
-    <x:workbookView xWindow="0" yWindow="0" windowWidth="22788" windowHeight="9552"/>
+    <x:workbookView xWindow="0" yWindow="0" windowWidth="22788" windowHeight="8256"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Sheet1" sheetId="1" r:id="rId4"/>
@@ -19,48 +19,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="84">
+<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="84">
   <x:si>
-    <x:t>SELECT 및 WHERE 통해 조건 일치하는 데이터 반환</x:t>
+    <x:t>새 게시물 추가</x:t>
   </x:si>
   <x:si>
-    <x:t>WLOP_MEMBER 테이블과 COMMENT 테이블 JOIN</x:t>
+    <x:t>리뷰 중복 추천 불가</x:t>
   </x:si>
   <x:si>
-    <x:t>WLOP_MEMBER 테이블의 REPORT_NUM INSERT</x:t>
-  </x:si>
-  <x:si>
-    <x:t>BILLBOARD 테이블에 수정할 게시물 내용 UPDATE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>LIKES 테이블에 reviews_like 값 INSERT</x:t>
-  </x:si>
-  <x:si>
-    <x:t>GROUP_BY INFO_CODE 및 ORDER_BY DESC</x:t>
-  </x:si>
-  <x:si>
-    <x:t>리뷰 추천</x:t>
-  </x:si>
-  <x:si>
-    <x:t>회원정보 수정</x:t>
-  </x:si>
-  <x:si>
-    <x:t>정보공유</x:t>
-  </x:si>
-  <x:si>
-    <x:t>게시글 추천</x:t>
-  </x:si>
-  <x:si>
-    <x:t>자유게시글</x:t>
-  </x:si>
-  <x:si>
-    <x:t>자유게시판</x:t>
-  </x:si>
-  <x:si>
-    <x:t>마이페이지</x:t>
-  </x:si>
-  <x:si>
-    <x:t>회원가입</x:t>
+    <x:t>블랙리스트 처리</x:t>
   </x:si>
   <x:si>
     <x:t>회원</x:t>
@@ -75,53 +42,88 @@
     <x:t>·</x:t>
   </x:si>
   <x:si>
-    <x:t>Pass Result</x:t>
+    <x:t>리뷰 추천</x:t>
   </x:si>
   <x:si>
-    <x:t>소분류</x:t>
+    <x:t>정보공유</x:t>
   </x:si>
   <x:si>
-    <x:t>탈퇴</x:t>
+    <x:t>회원정보 수정</x:t>
   </x:si>
   <x:si>
-    <x:t>대분류</x:t>
+    <x:t>회원가입</x:t>
   </x:si>
   <x:si>
-    <x:t>중분류</x:t>
+    <x:t>게시글 추천</x:t>
   </x:si>
   <x:si>
-    <x:t>비고</x:t>
+    <x:t>자유게시글</x:t>
   </x:si>
   <x:si>
-    <x:t>P/F</x:t>
+    <x:t>마이페이지</x:t>
   </x:si>
   <x:si>
-    <x:t>SELECT 및 WEHRE 조건문을 통해 입력한 정보와 기존 데이터 비교</x:t>
+    <x:t>자유게시판</x:t>
   </x:si>
   <x:si>
-    <x:t>블랙리스트가 된 회원이 작성한 모든 게시물 
-활성화 유뮤 N으로 일괄변경</x:t>
+    <x:t>등업조건 만족</x:t>
   </x:si>
   <x:si>
-    <x:t>duplicate error 발생 및 reviews_like 값 유지</x:t>
+    <x:t>리뷰게시글</x:t>
   </x:si>
   <x:si>
-    <x:t>BILLBOARD 테이블에서 삭제할 게시물 활성화 여부 UPDATE</x:t>
+    <x:t>자동등업</x:t>
   </x:si>
   <x:si>
-    <x:t>GROUP_BY reviews_like 및 ORDER_BY DESC</x:t>
+    <x:t>실행 순서</x:t>
   </x:si>
   <x:si>
-    <x:t>BLACKLIST 유무 UPDATE</x:t>
+    <x:t>관리자페이지</x:t>
+  </x:si>
+  <x:si>
+    <x:t>소개게시판</x:t>
+  </x:si>
+  <x:si>
+    <x:t>실제 결과</x:t>
+  </x:si>
+  <x:si>
+    <x:t>게시물 신고</x:t>
+  </x:si>
+  <x:si>
+    <x:t>게시물 게시</x:t>
+  </x:si>
+  <x:si>
+    <x:t>테스트 조건</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PASS</x:t>
+  </x:si>
+  <x:si>
+    <x:t>게시글 검색</x:t>
+  </x:si>
+  <x:si>
+    <x:t>작성댓글 조회</x:t>
+  </x:si>
+  <x:si>
+    <x:t>게시물 삭제</x:t>
+  </x:si>
+  <x:si>
+    <x:t>회원등급 변경</x:t>
+  </x:si>
+  <x:si>
+    <x:t>게시물 수정</x:t>
+  </x:si>
+  <x:si>
+    <x:t>로그인 필수</x:t>
+  </x:si>
+  <x:si>
+    <x:t>입력한 아이디 관련 회원정보 출력</x:t>
   </x:si>
   <x:si>
     <x:t>수정된 내용으로 게시내역 변경</x:t>
   </x:si>
   <x:si>
-    <x:t>게시물 활성화 여부 N으로 변경</x:t>
-  </x:si>
-  <x:si>
-    <x:t>board_likes 값 1로 변경</x:t>
+    <x:t>BLACKLIST 유무 UPDATE</x:t>
   </x:si>
   <x:si>
     <x:t>입력한 조건을 만족하는 게시글 반환</x:t>
@@ -133,16 +135,63 @@
     <x:t>리뷰 추천수가 많은 순으로 반환</x:t>
   </x:si>
   <x:si>
-    <x:t>입력한 아이디 관련 회원정보 출력</x:t>
+    <x:t>게시물 활성화 여부 N으로 변경</x:t>
   </x:si>
   <x:si>
-    <x:t>리뷰 중복 추천 불가</x:t>
+    <x:t>board_likes 값 1로 변경</x:t>
   </x:si>
   <x:si>
-    <x:t>블랙리스트 처리</x:t>
+    <x:t>WLOP_MEMEBER 테이블과
+INFORMATION, REVIEW, BILLBOARD, GOODSSHARE, REPORT, QNA 테이블 JOIN</x:t>
   </x:si>
   <x:si>
-    <x:t>새 게시물 추가</x:t>
+    <x:t>SELECT 및 WEHRE 조건문을 통해 입력한 정보와 기존 데이터 비교</x:t>
+  </x:si>
+  <x:si>
+    <x:t>블랙리스트가 된 회원이 작성한 모든 게시물 
+활성화 유뮤 N으로 일괄변경</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SELECT 및 WHERE 통해 조건 일치하는 데이터 반환</x:t>
+  </x:si>
+  <x:si>
+    <x:t>WLOP_MEMBER 테이블과 COMMENT 테이블 JOIN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BILLBOARD 테이블에 수정할 게시물 내용 UPDATE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>LIKES 테이블에 reviews_like 값 INSERT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>GROUP_BY INFO_CODE 및 ORDER_BY DESC</x:t>
+  </x:si>
+  <x:si>
+    <x:t>WLOP_MEMBER 테이블의 REPORT_NUM INSERT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MEMBERADMIN 테이블에서 회원상태 UPDATE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>LIKES 테이블에 board_likes 값 INSERT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>WLOP_MEMBER 테이블에 회원정보 INSERT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BILLBOARD 테이블에 게시물 내용 INSERT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Pass Result</x:t>
+  </x:si>
+  <x:si>
+    <x:t>duplicate error 발생 및 reviews_like 값 유지</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BILLBOARD 테이블에서 삭제할 게시물 활성화 여부 UPDATE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>GROUP_BY reviews_like 및 ORDER_BY DESC</x:t>
   </x:si>
   <x:si>
     <x:t>작성게시물 조회</x:t>
@@ -157,83 +206,10 @@
     <x:t>타인 게시물 조회</x:t>
   </x:si>
   <x:si>
-    <x:t>MEMBERADMIN 테이블에서 회원상태 UPDATE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>LIKES 테이블에 board_likes 값 INSERT</x:t>
-  </x:si>
-  <x:si>
-    <x:t>WLOP_MEMBER 테이블에 회원정보 INSERT</x:t>
-  </x:si>
-  <x:si>
-    <x:t>BILLBOARD 테이블에 게시물 내용 INSERT</x:t>
-  </x:si>
-  <x:si>
-    <x:t>WLOP_MEMEBER 테이블과
-INFORMATION, REVIEW, BILLBOARD, GOODSSHARE, REPORT, QNA 테이블 JOIN</x:t>
-  </x:si>
-  <x:si>
-    <x:t>작성댓글 조회</x:t>
-  </x:si>
-  <x:si>
-    <x:t>게시물 게시</x:t>
-  </x:si>
-  <x:si>
-    <x:t>게시글 검색</x:t>
-  </x:si>
-  <x:si>
-    <x:t>실제 결과</x:t>
-  </x:si>
-  <x:si>
-    <x:t>소개게시판</x:t>
-  </x:si>
-  <x:si>
-    <x:t>리뷰게시글</x:t>
-  </x:si>
-  <x:si>
-    <x:t>실행 순서</x:t>
-  </x:si>
-  <x:si>
-    <x:t>게시물 신고</x:t>
-  </x:si>
-  <x:si>
-    <x:t>등업조건 만족</x:t>
-  </x:si>
-  <x:si>
-    <x:t>테스트 조건</x:t>
-  </x:si>
-  <x:si>
-    <x:t>게시물 삭제</x:t>
-  </x:si>
-  <x:si>
-    <x:t>관리자페이지</x:t>
-  </x:si>
-  <x:si>
-    <x:t>자동등업</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PASS</x:t>
-  </x:si>
-  <x:si>
-    <x:t>로그인 필수</x:t>
-  </x:si>
-  <x:si>
-    <x:t>회원등급 변경</x:t>
-  </x:si>
-  <x:si>
-    <x:t>게시물 수정</x:t>
-  </x:si>
-  <x:si>
     <x:t>신고 게시물 처리</x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">신고 테이블에 </x:t>
-  </x:si>
-  <x:si>
-    <x:t>회원 데이터 내역 변경</x:t>
-  </x:si>
-  <x:si>
-    <x:t>내가 작성한 게시물 반환</x:t>
   </x:si>
   <x:si>
     <x:t>내가 작성한 댓글 반환</x:t>
@@ -242,10 +218,10 @@
     <x:t>동일 게시글 추천 기록X</x:t>
   </x:si>
   <x:si>
-    <x:t>관련 리뷰 많은 순으로 조회</x:t>
+    <x:t>내가 작성한 게시물 반환</x:t>
   </x:si>
   <x:si>
-    <x:t>회원테이블에 데이터 추가</x:t>
+    <x:t>관련 리뷰 많은 순으로 조회</x:t>
   </x:si>
   <x:si>
     <x:t>추천이 많은 순으로 조회</x:t>
@@ -254,25 +230,49 @@
     <x:t>동일 리뷰 추천 기록X</x:t>
   </x:si>
   <x:si>
-    <x:t>INFORMATION, REVIEW를 VIEW</x:t>
+    <x:t>회원 데이터 내역 변경</x:t>
+  </x:si>
+  <x:si>
+    <x:t>회원테이블에 데이터 추가</x:t>
+  </x:si>
+  <x:si>
+    <x:t>비고</x:t>
+  </x:si>
+  <x:si>
+    <x:t>대분류</x:t>
+  </x:si>
+  <x:si>
+    <x:t>소분류</x:t>
+  </x:si>
+  <x:si>
+    <x:t>중분류</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P/F</x:t>
+  </x:si>
+  <x:si>
+    <x:t>탈퇴</x:t>
+  </x:si>
+  <x:si>
+    <x:t>관련 리뷰가 많은 소개글을 내림차순으로 반환</x:t>
   </x:si>
   <x:si>
     <x:t>WLOP_MEMEBR 변경할 회원정보 UPDATE</x:t>
   </x:si>
   <x:si>
-    <x:t>관련 리뷰가 많은 소개글을 내림차순으로 반환</x:t>
+    <x:t>INFORMATION, REVIEW를 VIEW</x:t>
   </x:si>
   <x:si>
-    <x:t>신고된 게시물 활성화 유무 N으로 변경</x:t>
+    <x:t>MEMBER_GRADE 값 UPDATE</x:t>
   </x:si>
   <x:si>
     <x:t>회원상태 변경 및 게시물 활성화 유무 변경</x:t>
   </x:si>
   <x:si>
-    <x:t>MEMBER_GRADE 값 UPDATE</x:t>
+    <x:t>review_likes 값 1로 변경</x:t>
   </x:si>
   <x:si>
-    <x:t>review_likes 값 1로 변경</x:t>
+    <x:t>신고된 게시물 활성화 유무 N으로 변경</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -590,58 +590,6 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-          <x:alignment horizontal="center" vertical="center"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-          <x:alignment horizontal="center" vertical="center"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
         <x:xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
           <x:alignment horizontal="center" vertical="center"/>
           <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
@@ -662,32 +610,6 @@
       </mc:Choice>
       <mc:Fallback>
         <x:xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-          <x:alignment horizontal="center" vertical="center"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-          <x:alignment horizontal="center" vertical="center"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
           <x:alignment horizontal="center" vertical="center"/>
         </x:xf>
       </mc:Fallback>
@@ -741,6 +663,84 @@
       <mc:Fallback>
         <x:xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
           <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
         </x:xf>
       </mc:Fallback>
     </mc:AlternateContent>
@@ -1445,7 +1445,7 @@
   <x:dimension ref="A1:XFD51"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" topLeftCell="A1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <x:selection activeCell="G13" activeCellId="0" sqref="G13:G13"/>
+      <x:selection activeCell="G28" activeCellId="0" sqref="G28:G28"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="16.399999999999999"/>
@@ -17850,116 +17850,116 @@
     </x:row>
     <x:row r="2" spans="2:10" s="2" customFormat="1" ht="17.149999999999999">
       <x:c r="B2" s="3" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="C2" s="4" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="D2" s="4" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="E2" s="4" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="F2" s="4" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="G2" s="4" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="H2" s="4" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="I2" s="4" t="s">
         <x:v>21</x:v>
       </x:c>
-      <x:c r="C2" s="4" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="D2" s="4" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="E2" s="4" t="s">
-        <x:v>59</x:v>
-      </x:c>
-      <x:c r="F2" s="4" t="s">
-        <x:v>56</x:v>
-      </x:c>
-      <x:c r="G2" s="4" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="H2" s="4" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="I2" s="4" t="s">
-        <x:v>53</x:v>
-      </x:c>
       <x:c r="J2" s="5" t="s">
-        <x:v>23</x:v>
+        <x:v>71</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="2:10">
-      <x:c r="B3" s="14" t="s">
-        <x:v>14</x:v>
+      <x:c r="B3" s="10" t="s">
+        <x:v>3</x:v>
       </x:c>
       <x:c r="C3" s="9" t="s">
-        <x:v>13</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="D3" s="9" t="s">
-        <x:v>17</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="E3" s="9"/>
       <x:c r="F3" s="9" t="s">
-        <x:v>47</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="G3" s="9" t="s">
-        <x:v>74</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="H3" s="9" t="s">
-        <x:v>63</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="I3" s="9"/>
-      <x:c r="J3" s="15"/>
+      <x:c r="J3" s="11"/>
     </x:row>
     <x:row r="4" spans="2:10">
-      <x:c r="B4" s="14" t="s">
-        <x:v>14</x:v>
+      <x:c r="B4" s="10" t="s">
+        <x:v>3</x:v>
       </x:c>
       <x:c r="C4" s="9" t="s">
-        <x:v>16</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="D4" s="9" t="s">
-        <x:v>17</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="E4" s="9"/>
       <x:c r="F4" s="9" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="G4" s="9" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="H4" s="9" t="s">
         <x:v>25</x:v>
       </x:c>
-      <x:c r="G4" s="9" t="s">
-        <x:v>37</x:v>
-      </x:c>
-      <x:c r="H4" s="9" t="s">
-        <x:v>63</x:v>
-      </x:c>
       <x:c r="I4" s="9"/>
-      <x:c r="J4" s="15"/>
+      <x:c r="J4" s="11"/>
     </x:row>
     <x:row r="5" spans="2:10">
-      <x:c r="B5" s="14" t="s">
-        <x:v>14</x:v>
+      <x:c r="B5" s="10" t="s">
+        <x:v>3</x:v>
       </x:c>
       <x:c r="C5" s="9" t="s">
-        <x:v>12</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="D5" s="9" t="s">
-        <x:v>20</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="E5" s="9" t="s">
-        <x:v>64</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="F5" s="9" t="s">
-        <x:v>45</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="G5" s="9" t="s">
         <x:v>81</x:v>
       </x:c>
       <x:c r="H5" s="9" t="s">
-        <x:v>63</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="I5" s="9"/>
-      <x:c r="J5" s="15"/>
+      <x:c r="J5" s="11"/>
     </x:row>
     <x:row r="6" spans="2:10">
-      <x:c r="B6" s="14" t="s">
-        <x:v>14</x:v>
+      <x:c r="B6" s="10" t="s">
+        <x:v>3</x:v>
       </x:c>
       <x:c r="C6" s="9" t="s">
-        <x:v>12</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="D6" s="9" t="s">
-        <x:v>7</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="E6" s="9" t="s">
-        <x:v>64</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="F6" s="9" t="s">
         <x:v>78</x:v>
@@ -17968,13 +17968,13 @@
         <x:v>69</x:v>
       </x:c>
       <x:c r="H6" s="9" t="s">
-        <x:v>63</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="I6" s="9"/>
-      <x:c r="J6" s="15"/>
+      <x:c r="J6" s="11"/>
     </x:row>
     <x:row r="7" spans="2:10" hidden="1">
-      <x:c r="B7" s="14"/>
+      <x:c r="B7" s="10"/>
       <x:c r="C7" s="9"/>
       <x:c r="D7" s="9"/>
       <x:c r="E7" s="9"/>
@@ -17982,518 +17982,526 @@
       <x:c r="G7" s="9"/>
       <x:c r="H7" s="9"/>
       <x:c r="I7" s="9"/>
-      <x:c r="J7" s="15"/>
+      <x:c r="J7" s="11"/>
     </x:row>
     <x:row r="8" spans="2:10" s="1" customFormat="1">
       <x:c r="B8" s="16" t="s">
-        <x:v>14</x:v>
+        <x:v>3</x:v>
       </x:c>
-      <x:c r="C8" s="10" t="s">
-        <x:v>12</x:v>
+      <x:c r="C8" s="18" t="s">
+        <x:v>13</x:v>
       </x:c>
-      <x:c r="D8" s="10" t="s">
-        <x:v>41</x:v>
+      <x:c r="D8" s="18" t="s">
+        <x:v>57</x:v>
       </x:c>
-      <x:c r="E8" s="10"/>
-      <x:c r="F8" s="12" t="s">
-        <x:v>49</x:v>
+      <x:c r="E8" s="18"/>
+      <x:c r="F8" s="20" t="s">
+        <x:v>40</x:v>
       </x:c>
-      <x:c r="G8" s="10" t="s">
-        <x:v>70</x:v>
+      <x:c r="G8" s="18" t="s">
+        <x:v>65</x:v>
       </x:c>
-      <x:c r="H8" s="10" t="s">
-        <x:v>63</x:v>
+      <x:c r="H8" s="18" t="s">
+        <x:v>25</x:v>
       </x:c>
       <x:c r="I8" s="9"/>
-      <x:c r="J8" s="15"/>
+      <x:c r="J8" s="11"/>
     </x:row>
     <x:row r="9" spans="2:10">
       <x:c r="B9" s="17"/>
-      <x:c r="C9" s="11"/>
-      <x:c r="D9" s="11"/>
-      <x:c r="E9" s="10"/>
-      <x:c r="F9" s="13"/>
-      <x:c r="G9" s="11"/>
-      <x:c r="H9" s="11"/>
+      <x:c r="C9" s="19"/>
+      <x:c r="D9" s="19"/>
+      <x:c r="E9" s="18"/>
+      <x:c r="F9" s="21"/>
+      <x:c r="G9" s="19"/>
+      <x:c r="H9" s="19"/>
       <x:c r="I9" s="9"/>
-      <x:c r="J9" s="15"/>
+      <x:c r="J9" s="11"/>
     </x:row>
     <x:row r="10" spans="2:10">
-      <x:c r="B10" s="14" t="s">
-        <x:v>14</x:v>
+      <x:c r="B10" s="10" t="s">
+        <x:v>3</x:v>
       </x:c>
       <x:c r="C10" s="9" t="s">
-        <x:v>12</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="D10" s="9" t="s">
-        <x:v>50</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="E10" s="9"/>
       <x:c r="F10" s="9" t="s">
-        <x:v>1</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="G10" s="9" t="s">
-        <x:v>71</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="H10" s="9" t="s">
-        <x:v>63</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="I10" s="9"/>
-      <x:c r="J10" s="15"/>
+      <x:c r="J10" s="11"/>
     </x:row>
     <x:row r="11" spans="2:10">
-      <x:c r="B11" s="14" t="s">
-        <x:v>11</x:v>
+      <x:c r="B11" s="10" t="s">
+        <x:v>14</x:v>
       </x:c>
       <x:c r="C11" s="9" t="s">
-        <x:v>10</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="D11" s="9" t="s">
-        <x:v>51</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="E11" s="9"/>
       <x:c r="F11" s="9" t="s">
-        <x:v>48</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="G11" s="9" t="s">
-        <x:v>40</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="H11" s="9" t="s">
-        <x:v>63</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="I11" s="9"/>
-      <x:c r="J11" s="15"/>
+      <x:c r="J11" s="11"/>
     </x:row>
     <x:row r="12" spans="2:10">
-      <x:c r="B12" s="14" t="s">
-        <x:v>11</x:v>
+      <x:c r="B12" s="10" t="s">
+        <x:v>14</x:v>
       </x:c>
       <x:c r="C12" s="9" t="s">
-        <x:v>10</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="D12" s="9" t="s">
-        <x:v>66</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="E12" s="9"/>
       <x:c r="F12" s="9" t="s">
-        <x:v>3</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="G12" s="9" t="s">
-        <x:v>31</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="H12" s="9" t="s">
-        <x:v>63</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="I12" s="9"/>
-      <x:c r="J12" s="15"/>
+      <x:c r="J12" s="11"/>
     </x:row>
     <x:row r="13" spans="2:10">
-      <x:c r="B13" s="14" t="s">
-        <x:v>11</x:v>
+      <x:c r="B13" s="10" t="s">
+        <x:v>14</x:v>
       </x:c>
       <x:c r="C13" s="9" t="s">
-        <x:v>10</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="D13" s="9" t="s">
-        <x:v>60</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="E13" s="9"/>
       <x:c r="F13" s="9" t="s">
-        <x:v>28</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="G13" s="9" t="s">
-        <x:v>32</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="H13" s="9" t="s">
-        <x:v>63</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="I13" s="9"/>
-      <x:c r="J13" s="15"/>
+      <x:c r="J13" s="11"/>
     </x:row>
     <x:row r="14" spans="2:10" hidden="1">
-      <x:c r="B14" s="14" t="s">
-        <x:v>11</x:v>
+      <x:c r="B14" s="10" t="s">
+        <x:v>14</x:v>
       </x:c>
       <x:c r="C14" s="9" t="s">
-        <x:v>10</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="D14" s="9" t="s">
-        <x:v>57</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="E14" s="9"/>
       <x:c r="F14" s="9"/>
       <x:c r="G14" s="9" t="s">
-        <x:v>68</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="H14" s="9" t="s">
-        <x:v>63</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="I14" s="9"/>
-      <x:c r="J14" s="15"/>
+      <x:c r="J14" s="11"/>
     </x:row>
     <x:row r="15" spans="2:10">
-      <x:c r="B15" s="14" t="s">
+      <x:c r="B15" s="10" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="C15" s="9" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="C15" s="9" t="s">
-        <x:v>9</x:v>
-      </x:c>
       <x:c r="D15" s="9" t="s">
-        <x:v>9</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="E15" s="9" t="s">
-        <x:v>72</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="F15" s="9" t="s">
-        <x:v>46</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="G15" s="9" t="s">
-        <x:v>33</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="H15" s="9" t="s">
-        <x:v>63</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="I15" s="9"/>
-      <x:c r="J15" s="15"/>
+      <x:c r="J15" s="11"/>
     </x:row>
     <x:row r="16" spans="2:10" s="1" customFormat="1">
-      <x:c r="B16" s="14" t="s">
-        <x:v>11</x:v>
+      <x:c r="B16" s="10" t="s">
+        <x:v>14</x:v>
       </x:c>
       <x:c r="C16" s="9" t="s">
-        <x:v>10</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="D16" s="9" t="s">
-        <x:v>52</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="E16" s="9"/>
-      <x:c r="F16" s="18" t="s">
-        <x:v>0</x:v>
+      <x:c r="F16" s="12" t="s">
+        <x:v>43</x:v>
       </x:c>
       <x:c r="G16" s="9" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="H16" s="9" t="s">
-        <x:v>63</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="I16" s="9"/>
-      <x:c r="J16" s="15"/>
+      <x:c r="J16" s="11"/>
     </x:row>
     <x:row r="17" spans="2:10">
-      <x:c r="B17" s="14" t="s">
-        <x:v>11</x:v>
+      <x:c r="B17" s="10" t="s">
+        <x:v>14</x:v>
       </x:c>
       <x:c r="C17" s="9" t="s">
-        <x:v>10</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="D17" s="9" t="s">
-        <x:v>44</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="E17" s="9"/>
       <x:c r="F17" s="9" t="s">
-        <x:v>77</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="G17" s="9" t="s">
-        <x:v>35</x:v>
+        <x:v>36</x:v>
       </x:c>
-      <x:c r="H17" s="9"/>
+      <x:c r="H17" s="9" t="s">
+        <x:v>25</x:v>
+      </x:c>
       <x:c r="I17" s="9"/>
-      <x:c r="J17" s="15"/>
+      <x:c r="J17" s="11"/>
     </x:row>
     <x:row r="18" spans="2:10">
-      <x:c r="B18" s="14" t="s">
+      <x:c r="B18" s="10" t="s">
         <x:v>8</x:v>
       </x:c>
       <x:c r="C18" s="9" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D18" s="9" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="E18" s="9" t="s">
-        <x:v>76</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="F18" s="9" t="s">
-        <x:v>4</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="G18" s="9" t="s">
-        <x:v>83</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="H18" s="9" t="s">
-        <x:v>63</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="I18" s="9"/>
-      <x:c r="J18" s="15"/>
+      <x:c r="J18" s="11"/>
     </x:row>
     <x:row r="19" spans="2:10">
-      <x:c r="B19" s="14" t="s">
+      <x:c r="B19" s="10" t="s">
         <x:v>8</x:v>
       </x:c>
       <x:c r="C19" s="9" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D19" s="9" t="s">
-        <x:v>38</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="E19" s="9"/>
       <x:c r="F19" s="9" t="s">
-        <x:v>4</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="G19" s="9" t="s">
-        <x:v>27</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="H19" s="9" t="s">
-        <x:v>63</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="I19" s="9"/>
-      <x:c r="J19" s="15"/>
+      <x:c r="J19" s="11"/>
     </x:row>
     <x:row r="20" spans="2:10" s="1" customFormat="1">
-      <x:c r="B20" s="14" t="s">
+      <x:c r="B20" s="10" t="s">
         <x:v>8</x:v>
       </x:c>
       <x:c r="C20" s="9" t="s">
-        <x:v>54</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="D20" s="9" t="s">
-        <x:v>43</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="E20" s="9" t="s">
-        <x:v>73</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="F20" s="9" t="s">
-        <x:v>5</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="G20" s="9" t="s">
-        <x:v>79</x:v>
+        <x:v>77</x:v>
       </x:c>
-      <x:c r="H20" s="9"/>
+      <x:c r="H20" s="9" t="s">
+        <x:v>25</x:v>
+      </x:c>
       <x:c r="I20" s="9"/>
-      <x:c r="J20" s="15"/>
+      <x:c r="J20" s="11"/>
     </x:row>
     <x:row r="21" spans="2:10">
-      <x:c r="B21" s="14" t="s">
+      <x:c r="B21" s="10" t="s">
         <x:v>8</x:v>
       </x:c>
       <x:c r="C21" s="9" t="s">
-        <x:v>55</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="D21" s="9" t="s">
-        <x:v>42</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="E21" s="9" t="s">
-        <x:v>75</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="F21" s="9" t="s">
-        <x:v>29</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="G21" s="9" t="s">
-        <x:v>36</x:v>
+        <x:v>37</x:v>
       </x:c>
-      <x:c r="H21" s="9"/>
+      <x:c r="H21" s="9" t="s">
+        <x:v>25</x:v>
+      </x:c>
       <x:c r="I21" s="9"/>
-      <x:c r="J21" s="15"/>
+      <x:c r="J21" s="11"/>
     </x:row>
     <x:row r="22" spans="2:10">
-      <x:c r="B22" s="14" t="s">
-        <x:v>15</x:v>
+      <x:c r="B22" s="10" t="s">
+        <x:v>4</x:v>
       </x:c>
       <x:c r="C22" s="9" t="s">
-        <x:v>61</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="D22" s="9" t="s">
-        <x:v>67</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="E22" s="9"/>
       <x:c r="F22" s="9" t="s">
-        <x:v>2</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="G22" s="9" t="s">
-        <x:v>80</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="H22" s="9" t="s">
-        <x:v>63</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="I22" s="9"/>
-      <x:c r="J22" s="15"/>
+      <x:c r="J22" s="11"/>
     </x:row>
     <x:row r="23" spans="2:10">
       <x:c r="B23" s="16" t="s">
-        <x:v>15</x:v>
+        <x:v>4</x:v>
       </x:c>
-      <x:c r="C23" s="10" t="s">
-        <x:v>61</x:v>
+      <x:c r="C23" s="18" t="s">
+        <x:v>19</x:v>
       </x:c>
-      <x:c r="D23" s="10" t="s">
-        <x:v>39</x:v>
+      <x:c r="D23" s="18" t="s">
+        <x:v>2</x:v>
       </x:c>
-      <x:c r="E23" s="10"/>
-      <x:c r="F23" s="10" t="s">
-        <x:v>30</x:v>
+      <x:c r="E23" s="18"/>
+      <x:c r="F23" s="18" t="s">
+        <x:v>34</x:v>
       </x:c>
-      <x:c r="G23" s="12" t="s">
-        <x:v>26</x:v>
+      <x:c r="G23" s="20" t="s">
+        <x:v>42</x:v>
       </x:c>
-      <x:c r="H23" s="10" t="s">
-        <x:v>63</x:v>
+      <x:c r="H23" s="18" t="s">
+        <x:v>25</x:v>
       </x:c>
       <x:c r="I23" s="9"/>
-      <x:c r="J23" s="15"/>
+      <x:c r="J23" s="11"/>
     </x:row>
     <x:row r="24" spans="2:10">
       <x:c r="B24" s="16"/>
-      <x:c r="C24" s="10"/>
-      <x:c r="D24" s="10"/>
-      <x:c r="E24" s="10"/>
-      <x:c r="F24" s="10"/>
-      <x:c r="G24" s="12"/>
-      <x:c r="H24" s="10"/>
+      <x:c r="C24" s="18"/>
+      <x:c r="D24" s="18"/>
+      <x:c r="E24" s="18"/>
+      <x:c r="F24" s="18"/>
+      <x:c r="G24" s="20"/>
+      <x:c r="H24" s="18" t="s">
+        <x:v>25</x:v>
+      </x:c>
       <x:c r="I24" s="9"/>
-      <x:c r="J24" s="15"/>
+      <x:c r="J24" s="11"/>
     </x:row>
     <x:row r="25" spans="2:10">
-      <x:c r="B25" s="19" t="s">
+      <x:c r="B25" s="13" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="C25" s="14" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="D25" s="14" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="E25" s="14" t="s">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="C25" s="20" t="s">
-        <x:v>61</x:v>
+      <x:c r="F25" s="14" t="s">
+        <x:v>80</x:v>
       </x:c>
-      <x:c r="D25" s="20" t="s">
-        <x:v>62</x:v>
+      <x:c r="G25" s="14" t="s">
+        <x:v>29</x:v>
       </x:c>
-      <x:c r="E25" s="20" t="s">
-        <x:v>58</x:v>
+      <x:c r="H25" s="14" t="s">
+        <x:v>25</x:v>
       </x:c>
-      <x:c r="F25" s="20" t="s">
-        <x:v>82</x:v>
-      </x:c>
-      <x:c r="G25" s="20" t="s">
-        <x:v>65</x:v>
-      </x:c>
-      <x:c r="H25" s="20" t="s">
-        <x:v>63</x:v>
-      </x:c>
-      <x:c r="I25" s="20"/>
-      <x:c r="J25" s="21"/>
+      <x:c r="I25" s="14"/>
+      <x:c r="J25" s="15"/>
     </x:row>
     <x:row r="26" spans="2:10">
-      <x:c r="B26" s="18"/>
-      <x:c r="C26" s="18"/>
-      <x:c r="D26" s="18"/>
-      <x:c r="E26" s="18"/>
-      <x:c r="F26" s="18"/>
-      <x:c r="G26" s="18"/>
-      <x:c r="H26" s="18"/>
+      <x:c r="B26" s="12"/>
+      <x:c r="C26" s="12"/>
+      <x:c r="D26" s="12"/>
+      <x:c r="E26" s="12"/>
+      <x:c r="F26" s="12"/>
+      <x:c r="G26" s="12"/>
+      <x:c r="H26" s="12"/>
       <x:c r="I26" s="6"/>
       <x:c r="J26" s="6"/>
     </x:row>
     <x:row r="27" spans="2:10">
-      <x:c r="B27" s="18"/>
-      <x:c r="C27" s="18"/>
-      <x:c r="D27" s="18"/>
-      <x:c r="E27" s="18"/>
-      <x:c r="F27" s="18"/>
-      <x:c r="G27" s="18"/>
-      <x:c r="H27" s="18"/>
+      <x:c r="B27" s="12"/>
+      <x:c r="C27" s="12"/>
+      <x:c r="D27" s="12"/>
+      <x:c r="E27" s="12"/>
+      <x:c r="F27" s="12"/>
+      <x:c r="G27" s="12"/>
+      <x:c r="H27" s="12"/>
       <x:c r="I27" s="6"/>
       <x:c r="J27" s="6"/>
     </x:row>
     <x:row r="28" spans="2:10">
-      <x:c r="B28" s="18"/>
-      <x:c r="C28" s="18"/>
-      <x:c r="D28" s="18"/>
-      <x:c r="E28" s="18"/>
-      <x:c r="F28" s="18"/>
-      <x:c r="G28" s="18"/>
-      <x:c r="H28" s="18"/>
+      <x:c r="B28" s="12"/>
+      <x:c r="C28" s="12"/>
+      <x:c r="D28" s="12"/>
+      <x:c r="E28" s="12"/>
+      <x:c r="F28" s="12"/>
+      <x:c r="G28" s="12"/>
+      <x:c r="H28" s="12"/>
       <x:c r="I28" s="6"/>
       <x:c r="J28" s="6"/>
     </x:row>
     <x:row r="29" spans="2:10">
-      <x:c r="B29" s="18"/>
-      <x:c r="C29" s="18"/>
-      <x:c r="D29" s="18"/>
-      <x:c r="E29" s="18"/>
-      <x:c r="F29" s="18"/>
-      <x:c r="G29" s="18"/>
-      <x:c r="H29" s="18"/>
+      <x:c r="B29" s="12"/>
+      <x:c r="C29" s="12"/>
+      <x:c r="D29" s="12"/>
+      <x:c r="E29" s="12"/>
+      <x:c r="F29" s="12"/>
+      <x:c r="G29" s="12"/>
+      <x:c r="H29" s="12"/>
       <x:c r="I29" s="6"/>
       <x:c r="J29" s="6"/>
     </x:row>
     <x:row r="30" spans="2:10">
-      <x:c r="B30" s="18"/>
-      <x:c r="C30" s="18"/>
-      <x:c r="D30" s="18"/>
-      <x:c r="E30" s="18"/>
-      <x:c r="F30" s="18"/>
-      <x:c r="G30" s="18"/>
-      <x:c r="H30" s="18"/>
+      <x:c r="B30" s="12"/>
+      <x:c r="C30" s="12"/>
+      <x:c r="D30" s="12"/>
+      <x:c r="E30" s="12"/>
+      <x:c r="F30" s="12"/>
+      <x:c r="G30" s="12"/>
+      <x:c r="H30" s="12"/>
       <x:c r="I30" s="6"/>
       <x:c r="J30" s="6"/>
     </x:row>
     <x:row r="31" spans="2:10">
-      <x:c r="B31" s="18"/>
-      <x:c r="C31" s="18"/>
-      <x:c r="D31" s="18"/>
-      <x:c r="E31" s="18"/>
-      <x:c r="F31" s="18"/>
-      <x:c r="G31" s="18"/>
-      <x:c r="H31" s="18"/>
+      <x:c r="B31" s="12"/>
+      <x:c r="C31" s="12"/>
+      <x:c r="D31" s="12"/>
+      <x:c r="E31" s="12"/>
+      <x:c r="F31" s="12"/>
+      <x:c r="G31" s="12"/>
+      <x:c r="H31" s="12"/>
       <x:c r="I31" s="6"/>
       <x:c r="J31" s="6"/>
     </x:row>
     <x:row r="32" spans="2:10">
-      <x:c r="B32" s="18"/>
-      <x:c r="C32" s="18"/>
-      <x:c r="D32" s="18"/>
-      <x:c r="E32" s="18"/>
-      <x:c r="F32" s="18"/>
-      <x:c r="G32" s="18"/>
-      <x:c r="H32" s="18"/>
+      <x:c r="B32" s="12"/>
+      <x:c r="C32" s="12"/>
+      <x:c r="D32" s="12"/>
+      <x:c r="E32" s="12"/>
+      <x:c r="F32" s="12"/>
+      <x:c r="G32" s="12"/>
+      <x:c r="H32" s="12"/>
       <x:c r="I32" s="6"/>
       <x:c r="J32" s="6"/>
     </x:row>
     <x:row r="33" spans="2:10">
-      <x:c r="B33" s="18"/>
-      <x:c r="C33" s="18"/>
-      <x:c r="D33" s="18"/>
-      <x:c r="E33" s="18"/>
-      <x:c r="F33" s="18"/>
-      <x:c r="G33" s="18"/>
-      <x:c r="H33" s="18"/>
+      <x:c r="B33" s="12"/>
+      <x:c r="C33" s="12"/>
+      <x:c r="D33" s="12"/>
+      <x:c r="E33" s="12"/>
+      <x:c r="F33" s="12"/>
+      <x:c r="G33" s="12"/>
+      <x:c r="H33" s="12"/>
       <x:c r="I33" s="6"/>
       <x:c r="J33" s="6"/>
     </x:row>
     <x:row r="34" spans="2:10">
-      <x:c r="B34" s="18"/>
-      <x:c r="C34" s="18"/>
-      <x:c r="D34" s="18"/>
-      <x:c r="E34" s="18"/>
-      <x:c r="F34" s="18"/>
-      <x:c r="G34" s="18"/>
-      <x:c r="H34" s="18"/>
+      <x:c r="B34" s="12"/>
+      <x:c r="C34" s="12"/>
+      <x:c r="D34" s="12"/>
+      <x:c r="E34" s="12"/>
+      <x:c r="F34" s="12"/>
+      <x:c r="G34" s="12"/>
+      <x:c r="H34" s="12"/>
       <x:c r="I34" s="6"/>
       <x:c r="J34" s="6"/>
     </x:row>
     <x:row r="35" spans="2:10">
-      <x:c r="B35" s="18"/>
-      <x:c r="C35" s="18"/>
-      <x:c r="D35" s="18"/>
-      <x:c r="E35" s="18"/>
-      <x:c r="F35" s="18"/>
-      <x:c r="G35" s="18"/>
-      <x:c r="H35" s="18"/>
+      <x:c r="B35" s="12"/>
+      <x:c r="C35" s="12"/>
+      <x:c r="D35" s="12"/>
+      <x:c r="E35" s="12"/>
+      <x:c r="F35" s="12"/>
+      <x:c r="G35" s="12"/>
+      <x:c r="H35" s="12"/>
       <x:c r="I35" s="6"/>
       <x:c r="J35" s="6"/>
     </x:row>
     <x:row r="36" spans="2:10">
-      <x:c r="B36" s="18"/>
-      <x:c r="C36" s="18"/>
-      <x:c r="D36" s="18"/>
-      <x:c r="E36" s="18"/>
-      <x:c r="F36" s="18"/>
-      <x:c r="G36" s="18"/>
-      <x:c r="H36" s="18"/>
+      <x:c r="B36" s="12"/>
+      <x:c r="C36" s="12"/>
+      <x:c r="D36" s="12"/>
+      <x:c r="E36" s="12"/>
+      <x:c r="F36" s="12"/>
+      <x:c r="G36" s="12"/>
+      <x:c r="H36" s="12"/>
       <x:c r="I36" s="6"/>
       <x:c r="J36" s="6"/>
     </x:row>
@@ -18583,7 +18591,7 @@
       <x:c r="C46" s="9"/>
       <x:c r="D46" s="9"/>
       <x:c r="E46" s="9"/>
-      <x:c r="F46" s="10"/>
+      <x:c r="F46" s="18"/>
       <x:c r="G46" s="9"/>
       <x:c r="H46" s="9"/>
     </x:row>
@@ -18592,7 +18600,7 @@
       <x:c r="C47" s="9"/>
       <x:c r="D47" s="9"/>
       <x:c r="E47" s="9"/>
-      <x:c r="F47" s="10"/>
+      <x:c r="F47" s="18"/>
       <x:c r="G47" s="9"/>
       <x:c r="H47" s="9"/>
     </x:row>

</xml_diff>